<commit_message>
Data 10. 3. + export
</commit_message>
<xml_diff>
--- a/2024/MAVIS_objednavka_Boh_GVD24.xlsx
+++ b/2024/MAVIS_objednavka_Boh_GVD24.xlsx
@@ -112,13 +112,13 @@
     <t>Rokytnice u Přerova</t>
   </si>
   <si>
-    <t>1600 - 1649, 1652 - 1655, 1657 - 1659, 2020 - 2022, 2024, 2037, 2040 - 2043, 2800 - 2832, 2834, 2835, 2837, 2838, 2840, 2850, 2851, 2860 - 2869, 2871, 2872, 2874 - 2878, 2898 - 2900, 2915, 2921 - 2957, 2991 - 2997, 3000, 3050 - 3061, 3070 - 3085, 3090 - 3133, 3135, 3137, 3140 - 3160, 3170 - 3174, 3178, 3180 - 3196, 3300 - 3330, 3390, 3392, 3400 - 3438, 3497, 3498, 3900 - 3933, 3935, 3937, 3939 - 3952, 3954, 3956, 3960 - 3968, 3980, 3982, 3983, 3991, 4238, 4240 - 4242, 4244 - 4247, 12800 - 12853, 12860, 12861, 12900 - 12939, 13100 - 13142, 13144, 13146, 13171, 13173 - 13191, 13193 - 13196, 13198, 13199, 13201 - 13206, 13208 - 13223, 13300 - 13316, 13320 - 13328, 13330, 13332, 13334, 13340 - 13346, 13390, 13391, 13394, 13395, 13901 - 13918, 14200 - 14204, 14206 - 14252, 14261 - 14271, 21960 - 21966, 21969, 21971, 21974, 21976, 23100 - 23128, 23130, 23141, 23143, 23146, 23148, 23151 - 23153, 23155, 23157, 23190, 23191, 23300, 23301, 23352 - 23375, 28900 - 28906, 28908, 28910 - 28912, 28930 - 28935, 28937 - 28939, 28943, 28944, 28946, 28948 - 28950, 28951</t>
-  </si>
-  <si>
     <t>Mluvčí:</t>
   </si>
   <si>
     <t>vše nová (kromě 471)</t>
+  </si>
+  <si>
+    <t>1600 - 1655, 1657 - 1659, 2020 - 2022, 2024, 2037, 2040 - 2043, 2049, 2800 - 2832, 2834, 2835, 2837, 2838, 2840, 2850, 2851, 2860 - 2869, 2871, 2872, 2874 - 2878, 2898 - 2900, 2915, 2921 - 2957, 2991 - 2997, 3000, 3050 - 3061, 3070 - 3085, 3090 - 3133, 3135, 3137, 3139 - 3160, 3170 - 3174, 3178, 3180 - 3196, 3300 - 3330, 3390, 3392, 3400 - 3438, 3497, 3498, 3900 - 3933, 3935, 3937, 3939 - 3952, 3954, 3956, 3960 - 3968, 3980, 3982, 3983, 3991, 4238, 4240 - 4242, 4244 - 4247, 12800 - 12853, 12860, 12861, 12900 - 12939, 13100 - 13142, 13144, 13146, 13171, 13173 - 13191, 13193 - 13196, 13198, 13199, 13201 - 13206, 13208 - 13223, 13300 - 13316, 13320 - 13328, 13330, 13332, 13334, 13340 - 13346, 13390, 13391, 13394, 13395, 13901 - 13918, 14200 - 14204, 14206 - 14252, 14261 - 14271, 21960 - 21966, 21969, 21971, 21974, 21976, 23100 - 23128, 23130, 23141, 23143, 23146, 23148, 23151 - 23153, 23155, 23157, 23190, 23191, 23300, 23301, 23352 - 23375, 28900 - 28906, 28908, 28910 - 28912, 28930 - 28935, 28937 - 28939, 28943, 28944, 28946, 28948 - 28950, 28951</t>
   </si>
 </sst>
 </file>
@@ -497,8 +497,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -540,10 +540,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>32</v>
       </c>
       <c r="C5" s="2"/>
     </row>
@@ -662,7 +662,7 @@
       <c r="A19" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="3" t="s">
         <v>2</v>
       </c>
       <c r="C19" s="2"/>
@@ -681,9 +681,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="132" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" ht="118.8" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B22" s="4"/>
       <c r="C22" s="1"/>
@@ -916,7 +916,7 @@
   <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -958,10 +958,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>32</v>
       </c>
       <c r="C5" s="2"/>
     </row>
@@ -1080,7 +1080,7 @@
       <c r="A19" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="3" t="s">
         <v>2</v>
       </c>
       <c r="C19" s="2"/>

</xml_diff>

<commit_message>
Oprava chybně zadaných ZDD v KASO + export
</commit_message>
<xml_diff>
--- a/2024/MAVIS_objednavka_Boh_GVD24.xlsx
+++ b/2024/MAVIS_objednavka_Boh_GVD24.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\2024\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OIS\CD\Data\2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CEC580C-F9D1-4D92-9889-A20A3AF435F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5772"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Univ_razeni" sheetId="1" r:id="rId1"/>
@@ -118,13 +119,13 @@
     <t>vše nová (kromě 471)</t>
   </si>
   <si>
-    <t>1600 - 1655, 1657 - 1659, 2020 - 2022, 2024, 2037, 2040 - 2043, 2049, 2800 - 2832, 2834, 2835, 2837, 2838, 2840, 2850, 2851, 2860 - 2869, 2871, 2872, 2874 - 2878, 2898 - 2900, 2915, 2921 - 2957, 2991 - 2997, 3000, 3050 - 3061, 3070 - 3085, 3090 - 3133, 3135, 3137, 3139 - 3160, 3170 - 3174, 3178, 3180 - 3196, 3300 - 3330, 3390, 3392, 3400 - 3438, 3497, 3498, 3900 - 3933, 3935, 3937, 3939 - 3952, 3954, 3956, 3960 - 3968, 3980, 3982, 3983, 3991, 4238, 4240 - 4242, 4244 - 4247, 12800 - 12853, 12860, 12861, 12900 - 12939, 13100 - 13142, 13144, 13146, 13171, 13173 - 13191, 13193 - 13196, 13198, 13199, 13201 - 13206, 13208 - 13223, 13300 - 13316, 13320 - 13328, 13330, 13332, 13334, 13340 - 13346, 13390, 13391, 13394, 13395, 13901 - 13918, 14200 - 14204, 14206 - 14252, 14261 - 14271, 21960 - 21966, 21969, 21971, 21974, 21976, 23100 - 23128, 23130, 23141, 23143, 23146, 23148, 23151 - 23153, 23155, 23157, 23190, 23191, 23300, 23301, 23352 - 23375, 28900 - 28906, 28908, 28910 - 28912, 28930 - 28935, 28937 - 28939, 28943, 28944, 28946, 28948 - 28950, 28951</t>
+    <t>1600 - 1655, 1657 - 1659, 2020 - 2021, 2037, 2040 - 2043, 2049, 2800 - 2832, 2834, 2835, 2837, 2838, 2840, 2850, 2851, 2860 - 2869, 2871, 2872, 2874 - 2878, 2887, 2889, 2894, 2896, 2900, 2915, 2921 - 2957, 2991 - 2997, 3000, 3050 - 3061, 3068 - 3085, 3088 - 3133, 3135 - 3160, 3170 - 3174, 3178, 3180 - 3196, 3300 - 3330, 3390, 3392, 3400 - 3438, 3486, 3488, 3495, 3499, 3903, 3904, 3906, 3908, 3911, 3914, 3915, 3920 - 3923, 3926 - 3928, 3931 - 3934, 3937, 3939, 3941 - 3952, 3954, 3956, 3960, 3962, 3966, 3967, 3974 - 3985, 3987, 3991, 3999, 4238, 4240 - 4242, 4244 - 4246, 12800 - 12853, 12860, 12861, 12900 - 12939, 13100 - 13142, 13144, 13146, 13171, 13173 - 13191, 13193 - 13196, 13198, 13199, 13201 - 13205, 13207, 13208, 13210 - 13212, 13216 - 13218, 13220 - 13222, 13225 - 13230, 13300 - 13316, 13320 - 13328, 13330, 13332, 13334, 13340 - 13346, 13390, 13391, 13394, 13395, 13901 - 13912, 13914 - 13916, 13918, 13931, 13933, 13935, 13937, 13939, 14200 - 14202, 14204, 14205, 14207, 14208, 14210 - 14213, 14215 - 14243, 14247, 14249 - 14252, 14262, 14264, 14270, 14271, 14278, 14282, 14283, 21960 - 21966, 21969, 21971, 21974, 21976, 23100 - 23128, 23130, 23141, 23143, 23146, 23148, 23151 - 23153, 23155, 23157, 23190, 23191, 23300, 23301, 23352 - 23375, 28900 - 28906, 28908, 28910 - 28912, 28930 - 28935, 28937 - 28939, 28943, 28944, 28946, 28948 - 28950, 28951</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -209,9 +210,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motiv Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Kancelář">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -249,9 +250,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Kancelář">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -286,7 +287,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -321,7 +322,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Kancelář">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -494,33 +495,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="105.44140625" customWidth="1"/>
-    <col min="2" max="2" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="94.44140625" customWidth="1"/>
+    <col min="1" max="1" width="105.42578125" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="94.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="6"/>
       <c r="B2" s="3"/>
       <c r="C2" s="6"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -529,7 +530,7 @@
       </c>
       <c r="C3" s="6"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -538,7 +539,7 @@
       </c>
       <c r="C4" s="2"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>30</v>
       </c>
@@ -547,12 +548,12 @@
       </c>
       <c r="C5" s="2"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
       <c r="B6" s="4"/>
       <c r="C6" s="2"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
@@ -561,14 +562,14 @@
       </c>
       <c r="C7" s="2"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="2"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
@@ -577,7 +578,7 @@
       </c>
       <c r="C9" s="2"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
@@ -586,7 +587,7 @@
       </c>
       <c r="C10" s="6"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>16</v>
       </c>
@@ -595,7 +596,7 @@
       </c>
       <c r="C11" s="2"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>22</v>
       </c>
@@ -604,7 +605,7 @@
       </c>
       <c r="C12" s="2"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>17</v>
       </c>
@@ -613,7 +614,7 @@
       </c>
       <c r="C13" s="2"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>1</v>
       </c>
@@ -622,7 +623,7 @@
       </c>
       <c r="C14" s="2"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>18</v>
       </c>
@@ -631,7 +632,7 @@
       </c>
       <c r="C15" s="2"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>19</v>
       </c>
@@ -640,7 +641,7 @@
       </c>
       <c r="C16" s="2"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>3</v>
       </c>
@@ -649,7 +650,7 @@
       </c>
       <c r="C17" s="2"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>11</v>
       </c>
@@ -658,7 +659,7 @@
       </c>
       <c r="C18" s="2"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>23</v>
       </c>
@@ -667,12 +668,12 @@
       </c>
       <c r="C19" s="2"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="2"/>
       <c r="B20" s="4"/>
       <c r="C20" s="2"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
         <v>8</v>
       </c>
@@ -681,14 +682,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="118.8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" ht="153" x14ac:dyDescent="0.2">
       <c r="A22" s="9" t="s">
         <v>32</v>
       </c>
       <c r="B22" s="4"/>
       <c r="C22" s="1"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>26</v>
       </c>
@@ -699,7 +700,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>7</v>
       </c>
@@ -710,7 +711,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>7</v>
       </c>
@@ -721,7 +722,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>7</v>
       </c>
@@ -732,7 +733,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
         <v>7</v>
       </c>
@@ -743,7 +744,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="7" t="s">
         <v>7</v>
       </c>
@@ -754,7 +755,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>7</v>
       </c>
@@ -765,7 +766,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>7</v>
       </c>
@@ -776,7 +777,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="7" t="s">
         <v>7</v>
       </c>
@@ -787,7 +788,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="7" t="s">
         <v>7</v>
       </c>
@@ -798,7 +799,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="7" t="s">
         <v>7</v>
       </c>
@@ -809,7 +810,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>7</v>
       </c>
@@ -820,82 +821,82 @@
         <v>20</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="2"/>
       <c r="B35" s="4"/>
       <c r="C35" s="1"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="2"/>
       <c r="B36" s="4"/>
       <c r="C36" s="1"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="2"/>
       <c r="B37" s="4"/>
       <c r="C37" s="1"/>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="2"/>
       <c r="B38" s="4"/>
       <c r="C38" s="1"/>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="2"/>
       <c r="B39" s="4"/>
       <c r="C39" s="1"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="2"/>
       <c r="B40" s="4"/>
       <c r="C40" s="1"/>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="2"/>
       <c r="B41" s="4"/>
       <c r="C41" s="1"/>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="7"/>
       <c r="B42" s="4"/>
       <c r="C42" s="1"/>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="7"/>
       <c r="B43" s="4"/>
       <c r="C43" s="1"/>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="7"/>
       <c r="B44" s="4"/>
       <c r="C44" s="1"/>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="7"/>
       <c r="B45" s="4"/>
       <c r="C45" s="1"/>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="7"/>
       <c r="B46" s="4"/>
       <c r="C46" s="1"/>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="7"/>
       <c r="B47" s="4"/>
       <c r="C47" s="1"/>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="7"/>
       <c r="B48" s="4"/>
       <c r="C48" s="1"/>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="7"/>
       <c r="B49" s="4"/>
       <c r="C49" s="1"/>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="7"/>
       <c r="B50" s="4"/>
       <c r="C50" s="1"/>
@@ -912,33 +913,33 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="94.44140625" customWidth="1"/>
+    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="94.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="8"/>
       <c r="B2" s="3"/>
       <c r="C2" s="8"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -947,7 +948,7 @@
       </c>
       <c r="C3" s="8"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -956,7 +957,7 @@
       </c>
       <c r="C4" s="2"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>30</v>
       </c>
@@ -965,12 +966,12 @@
       </c>
       <c r="C5" s="2"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
       <c r="B6" s="4"/>
       <c r="C6" s="2"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
@@ -979,14 +980,14 @@
       </c>
       <c r="C7" s="2"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="2"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
@@ -995,7 +996,7 @@
       </c>
       <c r="C9" s="2"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
@@ -1004,7 +1005,7 @@
       </c>
       <c r="C10" s="8"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>16</v>
       </c>
@@ -1013,7 +1014,7 @@
       </c>
       <c r="C11" s="2"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>22</v>
       </c>
@@ -1022,7 +1023,7 @@
       </c>
       <c r="C12" s="2"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>17</v>
       </c>
@@ -1031,7 +1032,7 @@
       </c>
       <c r="C13" s="2"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>1</v>
       </c>
@@ -1040,7 +1041,7 @@
       </c>
       <c r="C14" s="2"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>18</v>
       </c>
@@ -1049,7 +1050,7 @@
       </c>
       <c r="C15" s="2"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>19</v>
       </c>
@@ -1058,7 +1059,7 @@
       </c>
       <c r="C16" s="2"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>3</v>
       </c>
@@ -1067,7 +1068,7 @@
       </c>
       <c r="C17" s="2"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>11</v>
       </c>
@@ -1076,7 +1077,7 @@
       </c>
       <c r="C18" s="2"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>23</v>
       </c>
@@ -1085,12 +1086,12 @@
       </c>
       <c r="C19" s="2"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="2"/>
       <c r="B20" s="4"/>
       <c r="C20" s="2"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="8" t="s">
         <v>8</v>
       </c>
@@ -1099,7 +1100,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>7</v>
       </c>
@@ -1110,7 +1111,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>7</v>
       </c>
@@ -1121,7 +1122,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>7</v>
       </c>
@@ -1132,7 +1133,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
         <v>26</v>
       </c>
@@ -1143,7 +1144,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="7" t="s">
         <v>26</v>
       </c>
@@ -1154,7 +1155,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
         <v>7</v>
       </c>
@@ -1165,7 +1166,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="7" t="s">
         <v>7</v>
       </c>
@@ -1176,7 +1177,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="7" t="s">
         <v>7</v>
       </c>
@@ -1187,7 +1188,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="7" t="s">
         <v>7</v>
       </c>
@@ -1198,17 +1199,17 @@
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="7"/>
       <c r="B31" s="4"/>
       <c r="C31" s="1"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="7"/>
       <c r="B32" s="4"/>
       <c r="C32" s="1"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="7"/>
       <c r="B33" s="4"/>
       <c r="C33" s="1"/>

</xml_diff>